<commit_message>
Zadanie 107 i 108
</commit_message>
<xml_diff>
--- a/matura.xlsx
+++ b/matura.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="28">
   <si>
     <t>Zadania</t>
   </si>
@@ -93,6 +93,12 @@
   </si>
   <si>
     <t>bez 5</t>
+  </si>
+  <si>
+    <t>Jedno z zadań zgadza sięz rozwiązaniem z CKE, ale nie zgadza się z odpowiedziami</t>
+  </si>
+  <si>
+    <t>W zadaniu 5 jest o 1 stacja za dużo</t>
   </si>
 </sst>
 </file>
@@ -550,8 +556,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:J56"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
-      <selection activeCell="D51" sqref="D51"/>
+    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
+      <selection activeCell="D53" sqref="D53"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -584,14 +590,14 @@
       </c>
       <c r="F1" s="2">
         <f>(H16-H15)/H16</f>
-        <v>0.79629629629629628</v>
+        <v>0.83333333333333337</v>
       </c>
       <c r="G1" t="s">
         <v>4</v>
       </c>
       <c r="H1" s="3">
         <f ca="1">H15/H11</f>
-        <v>0.22</v>
+        <v>0.21428571428571427</v>
       </c>
       <c r="I1" t="s">
         <v>5</v>
@@ -734,7 +740,7 @@
       </c>
       <c r="H11" s="7">
         <f ca="1">DATEDIF(TODAY(), H10, "d")</f>
-        <v>50</v>
+        <v>42</v>
       </c>
       <c r="I11" s="7"/>
     </row>
@@ -754,7 +760,7 @@
       </c>
       <c r="H12">
         <f ca="1">TRUNC(RAND()*55)+58</f>
-        <v>108</v>
+        <v>80</v>
       </c>
     </row>
     <row r="13" spans="2:10" x14ac:dyDescent="0.25">
@@ -806,7 +812,7 @@
       </c>
       <c r="H15">
         <f>COUNTBLANK(D2:D56)</f>
-        <v>11</v>
+        <v>9</v>
       </c>
     </row>
     <row r="16" spans="2:10" x14ac:dyDescent="0.25">
@@ -844,7 +850,7 @@
       </c>
       <c r="H17">
         <f>H16-H15</f>
-        <v>43</v>
+        <v>45</v>
       </c>
     </row>
     <row r="18" spans="2:8" x14ac:dyDescent="0.25">
@@ -1248,8 +1254,12 @@
       <c r="C51" s="5">
         <v>42773</v>
       </c>
-      <c r="D51" s="5"/>
-      <c r="E51" s="4"/>
+      <c r="D51" s="5">
+        <v>42823</v>
+      </c>
+      <c r="E51" s="4" t="s">
+        <v>26</v>
+      </c>
     </row>
     <row r="52" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B52" s="4">
@@ -1258,8 +1268,12 @@
       <c r="C52" s="5">
         <v>42774</v>
       </c>
-      <c r="D52" s="5"/>
-      <c r="E52" s="4"/>
+      <c r="D52" s="5">
+        <v>42823</v>
+      </c>
+      <c r="E52" s="4" t="s">
+        <v>27</v>
+      </c>
     </row>
     <row r="53" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B53" s="4">
@@ -1352,7 +1366,7 @@
       </c>
       <c r="M1" s="3">
         <f ca="1">J5/J7</f>
-        <v>3.0222222222222221</v>
+        <v>3.6756756756756759</v>
       </c>
     </row>
     <row r="2" spans="2:13" ht="20.25" thickBot="1" x14ac:dyDescent="0.35">
@@ -1455,7 +1469,7 @@
       </c>
       <c r="J7" s="7">
         <f ca="1">J6-TODAY()</f>
-        <v>45</v>
+        <v>37</v>
       </c>
     </row>
     <row r="8" spans="2:13" x14ac:dyDescent="0.25">

</xml_diff>